<commit_message>
feat(quotes.xlsx): add new quotes
</commit_message>
<xml_diff>
--- a/data_lunch_app/quotes.xlsx
+++ b/data_lunch_app/quotes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michi/Desktop/data-lunch/data_lunch_app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{92CF5FB3-08D5-F64A-BA00-745D3DAEA4A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECB5AB45-B06C-3D40-9E31-60EBD5CC70F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="620" yWindow="500" windowWidth="31960" windowHeight="18740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="group" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="139">
   <si>
     <t>“Never eat more than you can life.”</t>
   </si>
@@ -392,6 +392,51 @@
   </si>
   <si>
     <t>author</t>
+  </si>
+  <si>
+    <t>Dr. Mark Hyman</t>
+  </si>
+  <si>
+    <t>Anthelme Brillat-Savarin</t>
+  </si>
+  <si>
+    <t>José Andrés</t>
+  </si>
+  <si>
+    <t>Unknown</t>
+  </si>
+  <si>
+    <t>Jamie Oliver</t>
+  </si>
+  <si>
+    <t>Sheila Graham</t>
+  </si>
+  <si>
+    <t>"Food is not just fuel, it's information. It talks to your DNA and tells it what to do."</t>
+  </si>
+  <si>
+    <t>"The discovery of a new dish does more for human happiness than the discovery of a new star."</t>
+  </si>
+  <si>
+    <t>"Food is memories."</t>
+  </si>
+  <si>
+    <t>"Good bread is the most fundamentally satisfying of all foods; and good bread with fresh butter, the greatest of feasts."</t>
+  </si>
+  <si>
+    <t>"Food is the ingredient that binds us together."</t>
+  </si>
+  <si>
+    <t>"If you can eat with mates or friends or family, I mean, it's such a brilliant thing isn't it? If you feel really rubbish and you have a nice bit of food it makes you feel good, you know?"</t>
+  </si>
+  <si>
+    <t>"Food is the most primitive form of comfort."</t>
+  </si>
+  <si>
+    <t>"Food is the ultimate equalizer. It doesn't matter who you are or where you come from, everyone has to eat."</t>
+  </si>
+  <si>
+    <t>"Food is love made visible."</t>
   </si>
 </sst>
 </file>
@@ -770,10 +815,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B65"/>
+  <dimension ref="A1:B74"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="A66" sqref="A66:B74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1302,6 +1347,78 @@
         <v>121</v>
       </c>
     </row>
+    <row r="66" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>130</v>
+      </c>
+      <c r="B66" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>131</v>
+      </c>
+      <c r="B67" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>132</v>
+      </c>
+      <c r="B68" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>133</v>
+      </c>
+      <c r="B69" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>134</v>
+      </c>
+      <c r="B70" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>135</v>
+      </c>
+      <c r="B71" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>136</v>
+      </c>
+      <c r="B72" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>137</v>
+      </c>
+      <c r="B73" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>138</v>
+      </c>
+      <c r="B74" t="s">
+        <v>127</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>